<commit_message>
Done with Service and Promo Management
</commit_message>
<xml_diff>
--- a/ClickNStyle Documents/System Status  and Info.xlsx
+++ b/ClickNStyle Documents/System Status  and Info.xlsx
@@ -341,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="37">
   <si>
     <t>Phase #</t>
   </si>
@@ -461,7 +461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +490,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +509,11 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -628,10 +640,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,7 +672,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -668,8 +687,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,30 +711,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -719,8 +729,18 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -991,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1002,7 +1022,7 @@
   <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,28 +1036,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="30">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1061,13 +1081,13 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="30">
-        <v>42661</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="29">
+        <v>42672</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1081,14 +1101,14 @@
         <v>23</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="22"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1102,12 +1122,12 @@
         <v>23</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="22"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
@@ -1117,12 +1137,12 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="22"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1132,12 +1152,12 @@
       </c>
       <c r="G6" s="9"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="15"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1150,9 +1170,9 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="22"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1164,14 +1184,14 @@
         <v>23</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="22"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
@@ -1185,12 +1205,12 @@
         <v>23</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="22"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
@@ -1204,12 +1224,12 @@
         <v>23</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="22"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1219,12 +1239,12 @@
         <v>23</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="22"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
@@ -1237,9 +1257,9 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="22"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1251,12 +1271,14 @@
         <v>23</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="22"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1270,13 +1292,13 @@
         <v>23</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="22"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1290,12 +1312,12 @@
         <v>23</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
@@ -1305,12 +1327,12 @@
         <v>23</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
@@ -1323,9 +1345,9 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1337,12 +1359,14 @@
         <v>23</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="9" t="s">
         <v>15</v>
       </c>
@@ -1356,12 +1380,12 @@
         <v>23</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="22"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1373,12 +1397,12 @@
         <v>23</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="22"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
@@ -1388,12 +1412,12 @@
         <v>23</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="22"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="9" t="s">
         <v>5</v>
       </c>
@@ -1406,9 +1430,9 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="22"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="16" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1423,9 +1447,9 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="22"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
@@ -1442,9 +1466,9 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="22"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="9" t="s">
         <v>16</v>
       </c>
@@ -1459,9 +1483,9 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="22"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
@@ -1474,9 +1498,9 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="22"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1489,9 +1513,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="22"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="16" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1506,9 +1530,9 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="22"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1525,9 +1549,9 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="22"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="9" t="s">
         <v>16</v>
       </c>
@@ -1540,9 +1564,9 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="22"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
@@ -1555,9 +1579,9 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="22"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="9" t="s">
         <v>5</v>
       </c>
@@ -1570,9 +1594,9 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="22"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="16" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -1587,9 +1611,9 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="22"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
@@ -1604,9 +1628,9 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="22"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="9" t="s">
         <v>16</v>
       </c>
@@ -1619,9 +1643,9 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="22"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="9" t="s">
         <v>4</v>
       </c>
@@ -1634,9 +1658,9 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="22"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="9" t="s">
         <v>5</v>
       </c>
@@ -1649,9 +1673,9 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="22"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="16" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -1666,9 +1690,9 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="22"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1681,9 +1705,9 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="22"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="17"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="9" t="s">
         <v>16</v>
       </c>
@@ -1696,9 +1720,9 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="22"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
@@ -1711,9 +1735,9 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="23"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -1748,13 +1772,13 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -1769,9 +1793,9 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="9" t="s">
         <v>15</v>
       </c>
@@ -1788,9 +1812,9 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="22"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="9" t="s">
         <v>16</v>
       </c>
@@ -1803,9 +1827,9 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="22"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="17"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="9" t="s">
         <v>4</v>
       </c>
@@ -1820,9 +1844,9 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="22"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="17"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -1833,9 +1857,9 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="22"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="16" t="s">
+      <c r="A49" s="19"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -1848,9 +1872,9 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="22"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="17"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="9" t="s">
         <v>15</v>
       </c>
@@ -1863,9 +1887,9 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="22"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="17"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="9" t="s">
         <v>16</v>
       </c>
@@ -1876,9 +1900,9 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="22"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="17"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="9" t="s">
         <v>4</v>
       </c>
@@ -1889,9 +1913,9 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="22"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="17"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="6" t="s">
         <v>5</v>
       </c>
@@ -1902,9 +1926,9 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="22"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="16" t="s">
+      <c r="A54" s="19"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -1919,9 +1943,9 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="22"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="24"/>
       <c r="D55" s="9" t="s">
         <v>15</v>
       </c>
@@ -1936,9 +1960,9 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="22"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="17"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="24"/>
       <c r="D56" s="9" t="s">
         <v>16</v>
       </c>
@@ -1953,9 +1977,9 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="22"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="17"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="24"/>
       <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
@@ -1968,9 +1992,9 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="22"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="17"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
@@ -1981,9 +2005,9 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="22"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="16" t="s">
+      <c r="A59" s="19"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -1996,9 +2020,9 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="22"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="17"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="9" t="s">
         <v>15</v>
       </c>
@@ -2009,9 +2033,9 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="22"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="17"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="9" t="s">
         <v>16</v>
       </c>
@@ -2022,9 +2046,9 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="22"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="17"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="9" t="s">
         <v>4</v>
       </c>
@@ -2035,9 +2059,9 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="22"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="17"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2048,9 +2072,9 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="22"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="24" t="s">
+      <c r="A64" s="19"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -2063,9 +2087,9 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="22"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="9" t="s">
         <v>15</v>
       </c>
@@ -2080,9 +2104,9 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="22"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="9" t="s">
         <v>16</v>
       </c>
@@ -2095,9 +2119,9 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="22"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="25"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="9" t="s">
         <v>4</v>
       </c>
@@ -2108,9 +2132,9 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="22"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="26"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="23"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -2121,9 +2145,9 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="22"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="16" t="s">
+      <c r="A69" s="19"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15" t="s">
         <v>32</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -2136,9 +2160,9 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="22"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="17"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="24"/>
       <c r="D70" s="9" t="s">
         <v>15</v>
       </c>
@@ -2149,9 +2173,9 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="22"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="24"/>
       <c r="D71" s="9" t="s">
         <v>16</v>
       </c>
@@ -2162,9 +2186,9 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="22"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="17"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="24"/>
       <c r="D72" s="9" t="s">
         <v>4</v>
       </c>
@@ -2175,9 +2199,9 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="22"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="17"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="24"/>
       <c r="D73" s="6" t="s">
         <v>5</v>
       </c>
@@ -2188,9 +2212,9 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="22"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="16" t="s">
+      <c r="A74" s="19"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -2206,9 +2230,9 @@
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="22"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="17"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="9" t="s">
         <v>15</v>
       </c>
@@ -2222,9 +2246,9 @@
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="22"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="17"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="24"/>
       <c r="D76" s="9" t="s">
         <v>16</v>
       </c>
@@ -2238,9 +2262,9 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="22"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="17"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="24"/>
       <c r="D77" s="9" t="s">
         <v>4</v>
       </c>
@@ -2254,9 +2278,9 @@
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="23"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="9" t="s">
         <v>5</v>
       </c>
@@ -2434,7 +2458,18 @@
       <c r="I94" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="J18:J21"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="B44:B78"/>
     <mergeCell ref="A44:A78"/>
@@ -2451,15 +2486,6 @@
     <mergeCell ref="A3:A42"/>
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="J8:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Announcement and Staff User management module
</commit_message>
<xml_diff>
--- a/ClickNStyle Documents/System Status  and Info.xlsx
+++ b/ClickNStyle Documents/System Status  and Info.xlsx
@@ -341,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="37">
   <si>
     <t>Phase #</t>
   </si>
@@ -672,6 +672,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -679,63 +736,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1036,28 +1036,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="30">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1081,13 +1081,13 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="29">
         <v>42672</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1101,14 +1101,14 @@
         <v>23</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="24"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1122,12 +1122,12 @@
         <v>23</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="24"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
@@ -1137,12 +1137,12 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="24"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G6" s="9"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="15"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1170,9 +1170,9 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="24"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1184,14 +1184,14 @@
         <v>23</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="24"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
@@ -1205,12 +1205,12 @@
         <v>23</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="24"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
@@ -1224,12 +1224,12 @@
         <v>23</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="24"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1239,12 +1239,12 @@
         <v>23</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="24"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,9 +1257,9 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="24"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1271,14 +1271,14 @@
         <v>23</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="24"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1292,13 +1292,13 @@
         <v>23</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="24"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1312,12 +1312,12 @@
         <v>23</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="24"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
@@ -1327,12 +1327,12 @@
         <v>23</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="24"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
@@ -1345,9 +1345,9 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="24"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1359,14 +1359,14 @@
         <v>23</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="24"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="9" t="s">
         <v>15</v>
       </c>
@@ -1380,12 +1380,12 @@
         <v>23</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="14"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="24"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1397,12 +1397,12 @@
         <v>23</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="24"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
@@ -1412,12 +1412,12 @@
         <v>23</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="15"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="24"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="9" t="s">
         <v>5</v>
       </c>
@@ -1430,9 +1430,9 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="24"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="16" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1444,14 +1444,14 @@
         <v>23</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="24"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
@@ -1465,12 +1465,12 @@
         <v>23</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="14"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="24"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="9" t="s">
         <v>16</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>23</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="24"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
@@ -1497,12 +1497,12 @@
         <v>23</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="24"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1515,9 +1515,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="24"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="16" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1529,12 +1529,14 @@
         <v>23</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="J28" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="24"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1548,12 +1550,12 @@
         <v>23</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="24"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="9" t="s">
         <v>16</v>
       </c>
@@ -1563,12 +1565,12 @@
         <v>23</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="24"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
@@ -1578,12 +1580,12 @@
         <v>23</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="J31" s="34"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="24"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="9" t="s">
         <v>5</v>
       </c>
@@ -1596,9 +1598,9 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="24"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="16" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -1613,9 +1615,9 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="24"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
@@ -1630,9 +1632,9 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="24"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="9" t="s">
         <v>16</v>
       </c>
@@ -1645,9 +1647,9 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="24"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="9" t="s">
         <v>4</v>
       </c>
@@ -1660,9 +1662,9 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="24"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="9" t="s">
         <v>5</v>
       </c>
@@ -1675,9 +1677,9 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="24"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="16" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -1689,12 +1691,14 @@
         <v>23</v>
       </c>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="J38" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="24"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1704,12 +1708,12 @@
         <v>23</v>
       </c>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="24"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="17"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="9" t="s">
         <v>16</v>
       </c>
@@ -1719,12 +1723,12 @@
         <v>23</v>
       </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="24"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
@@ -1734,12 +1738,12 @@
         <v>23</v>
       </c>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="34"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="25"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -1774,13 +1778,13 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -1795,9 +1799,9 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="24"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="9" t="s">
         <v>15</v>
       </c>
@@ -1814,9 +1818,9 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="24"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="9" t="s">
         <v>16</v>
       </c>
@@ -1829,9 +1833,9 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="24"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="17"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="9" t="s">
         <v>4</v>
       </c>
@@ -1846,9 +1850,9 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="24"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="17"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -1859,9 +1863,9 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="24"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="16" t="s">
+      <c r="A49" s="19"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -1874,9 +1878,9 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="24"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="17"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="9" t="s">
         <v>15</v>
       </c>
@@ -1889,9 +1893,9 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="24"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="17"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="9" t="s">
         <v>16</v>
       </c>
@@ -1902,9 +1906,9 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="24"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="17"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="9" t="s">
         <v>4</v>
       </c>
@@ -1915,9 +1919,9 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="24"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="17"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="6" t="s">
         <v>5</v>
       </c>
@@ -1928,9 +1932,9 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="24"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="16" t="s">
+      <c r="A54" s="19"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -1945,9 +1949,9 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="24"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="24"/>
       <c r="D55" s="9" t="s">
         <v>15</v>
       </c>
@@ -1962,9 +1966,9 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="24"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="17"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="24"/>
       <c r="D56" s="9" t="s">
         <v>16</v>
       </c>
@@ -1979,9 +1983,9 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="24"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="17"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="24"/>
       <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
@@ -1994,9 +1998,9 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="24"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="17"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
@@ -2007,9 +2011,9 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="24"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="16" t="s">
+      <c r="A59" s="19"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -2022,9 +2026,9 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="24"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="17"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="9" t="s">
         <v>15</v>
       </c>
@@ -2035,9 +2039,9 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="24"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="17"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="9" t="s">
         <v>16</v>
       </c>
@@ -2048,9 +2052,9 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="24"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="17"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="9" t="s">
         <v>4</v>
       </c>
@@ -2061,9 +2065,9 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="24"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="17"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2074,9 +2078,9 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="24"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="26" t="s">
+      <c r="A64" s="19"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -2089,9 +2093,9 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="24"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="27"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="9" t="s">
         <v>15</v>
       </c>
@@ -2106,9 +2110,9 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="24"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="9" t="s">
         <v>16</v>
       </c>
@@ -2121,9 +2125,9 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="24"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="9" t="s">
         <v>4</v>
       </c>
@@ -2134,9 +2138,9 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="24"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="28"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="23"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -2147,9 +2151,9 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="24"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="16" t="s">
+      <c r="A69" s="19"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15" t="s">
         <v>32</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -2162,9 +2166,9 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="24"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="17"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="24"/>
       <c r="D70" s="9" t="s">
         <v>15</v>
       </c>
@@ -2175,9 +2179,9 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="24"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="24"/>
       <c r="D71" s="9" t="s">
         <v>16</v>
       </c>
@@ -2188,9 +2192,9 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="24"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="17"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="24"/>
       <c r="D72" s="9" t="s">
         <v>4</v>
       </c>
@@ -2201,9 +2205,9 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="24"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="17"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="24"/>
       <c r="D73" s="6" t="s">
         <v>5</v>
       </c>
@@ -2214,9 +2218,9 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="24"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="16" t="s">
+      <c r="A74" s="19"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -2232,9 +2236,9 @@
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="24"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="17"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="9" t="s">
         <v>15</v>
       </c>
@@ -2248,9 +2252,9 @@
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="24"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="17"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="24"/>
       <c r="D76" s="9" t="s">
         <v>16</v>
       </c>
@@ -2264,9 +2268,9 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="24"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="17"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="24"/>
       <c r="D77" s="9" t="s">
         <v>4</v>
       </c>
@@ -2280,9 +2284,9 @@
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="25"/>
-      <c r="B78" s="22"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="9" t="s">
         <v>5</v>
       </c>
@@ -2460,7 +2464,21 @@
       <c r="I94" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="J38:J41"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="B44:B78"/>
     <mergeCell ref="A44:A78"/>
@@ -2477,18 +2495,6 @@
     <mergeCell ref="A3:A42"/>
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="J23:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Staff users management
</commit_message>
<xml_diff>
--- a/ClickNStyle Documents/System Status  and Info.xlsx
+++ b/ClickNStyle Documents/System Status  and Info.xlsx
@@ -341,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="37">
   <si>
     <t>Phase #</t>
   </si>
@@ -672,15 +672,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,12 +720,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,15 +736,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38:J41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1036,28 +1036,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:11" ht="30">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1081,13 +1081,13 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="32">
         <v>42672</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1101,14 +1101,14 @@
         <v>23</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="19"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1122,12 +1122,12 @@
         <v>23</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="33"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="19"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="24"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
@@ -1137,12 +1137,12 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="33"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="19"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G6" s="9"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="34"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="19"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="25"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1170,9 +1170,9 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="19"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1184,14 +1184,14 @@
         <v>23</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="19"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
@@ -1205,12 +1205,12 @@
         <v>23</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="33"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="19"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
@@ -1224,12 +1224,12 @@
         <v>23</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="19"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1239,12 +1239,12 @@
         <v>23</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="34"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="19"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,9 +1257,9 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="19"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1271,14 +1271,14 @@
         <v>23</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="19"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1292,13 +1292,13 @@
         <v>23</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="19"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1312,12 +1312,12 @@
         <v>23</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="19"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
@@ -1327,12 +1327,12 @@
         <v>23</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="34"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="19"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
@@ -1345,9 +1345,9 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="19"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="15" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1359,14 +1359,14 @@
         <v>23</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="19"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="9" t="s">
         <v>15</v>
       </c>
@@ -1380,12 +1380,12 @@
         <v>23</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="33"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="19"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1397,12 +1397,12 @@
         <v>23</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="33"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="19"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
@@ -1412,12 +1412,12 @@
         <v>23</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="34"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="19"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="9" t="s">
         <v>5</v>
       </c>
@@ -1430,9 +1430,9 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="19"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="15" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1444,14 +1444,14 @@
         <v>23</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="32" t="s">
+      <c r="J23" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="19"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
@@ -1465,12 +1465,12 @@
         <v>23</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="33"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="19"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="24"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="9" t="s">
         <v>16</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>23</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="33"/>
+      <c r="J25" s="14"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="19"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
@@ -1497,12 +1497,12 @@
         <v>23</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="34"/>
+      <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="19"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1515,9 +1515,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="19"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="15" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1529,14 +1529,14 @@
         <v>23</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="32" t="s">
+      <c r="J28" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="19"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="24"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1550,12 +1550,12 @@
         <v>23</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="33"/>
+      <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="19"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="9" t="s">
         <v>16</v>
       </c>
@@ -1565,12 +1565,12 @@
         <v>23</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="33"/>
+      <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="19"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="24"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
@@ -1580,12 +1580,12 @@
         <v>23</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="34"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="19"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="9" t="s">
         <v>5</v>
       </c>
@@ -1598,9 +1598,9 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="19"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -1612,12 +1612,14 @@
         <v>23</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="19"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="24"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
@@ -1629,12 +1631,12 @@
         <v>23</v>
       </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="19"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="24"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="9" t="s">
         <v>16</v>
       </c>
@@ -1644,12 +1646,12 @@
         <v>23</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="14"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="19"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="9" t="s">
         <v>4</v>
       </c>
@@ -1659,12 +1661,12 @@
         <v>23</v>
       </c>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="19"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="9" t="s">
         <v>5</v>
       </c>
@@ -1677,9 +1679,9 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="19"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="15" t="s">
+      <c r="A38" s="24"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -1691,14 +1693,14 @@
         <v>23</v>
       </c>
       <c r="I38" s="1"/>
-      <c r="J38" s="32" t="s">
+      <c r="J38" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="19"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="17"/>
       <c r="D39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1708,12 +1710,12 @@
         <v>23</v>
       </c>
       <c r="I39" s="1"/>
-      <c r="J39" s="33"/>
+      <c r="J39" s="14"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="19"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="24"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="9" t="s">
         <v>16</v>
       </c>
@@ -1723,12 +1725,12 @@
         <v>23</v>
       </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="33"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="19"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="24"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
@@ -1738,12 +1740,12 @@
         <v>23</v>
       </c>
       <c r="I41" s="1"/>
-      <c r="J41" s="34"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="20"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="24"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -1778,13 +1780,13 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -1799,9 +1801,9 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="19"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="24"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="17"/>
       <c r="D45" s="9" t="s">
         <v>15</v>
       </c>
@@ -1818,9 +1820,9 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="19"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="24"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="9" t="s">
         <v>16</v>
       </c>
@@ -1833,9 +1835,9 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="19"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="24"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="9" t="s">
         <v>4</v>
       </c>
@@ -1850,9 +1852,9 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="19"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="24"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -1863,9 +1865,9 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="19"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="15" t="s">
+      <c r="A49" s="24"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -1878,9 +1880,9 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="19"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="24"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="9" t="s">
         <v>15</v>
       </c>
@@ -1893,9 +1895,9 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="19"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="24"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="17"/>
       <c r="D51" s="9" t="s">
         <v>16</v>
       </c>
@@ -1906,9 +1908,9 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="19"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="24"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="17"/>
       <c r="D52" s="9" t="s">
         <v>4</v>
       </c>
@@ -1919,9 +1921,9 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="19"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="24"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="17"/>
       <c r="D53" s="6" t="s">
         <v>5</v>
       </c>
@@ -1932,9 +1934,9 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="19"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="15" t="s">
+      <c r="A54" s="24"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -1949,9 +1951,9 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="19"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="24"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="9" t="s">
         <v>15</v>
       </c>
@@ -1966,9 +1968,9 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="19"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="24"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="17"/>
       <c r="D56" s="9" t="s">
         <v>16</v>
       </c>
@@ -1983,9 +1985,9 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="19"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="24"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="17"/>
       <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
@@ -1998,9 +2000,9 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="19"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="24"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="17"/>
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
@@ -2011,9 +2013,9 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="19"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="15" t="s">
+      <c r="A59" s="24"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -2026,9 +2028,9 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="19"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="24"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="17"/>
       <c r="D60" s="9" t="s">
         <v>15</v>
       </c>
@@ -2039,9 +2041,9 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="19"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="24"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="17"/>
       <c r="D61" s="9" t="s">
         <v>16</v>
       </c>
@@ -2052,9 +2054,9 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="19"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="24"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="17"/>
       <c r="D62" s="9" t="s">
         <v>4</v>
       </c>
@@ -2065,9 +2067,9 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="19"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="24"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="17"/>
       <c r="D63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2078,9 +2080,9 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="19"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="21" t="s">
+      <c r="A64" s="24"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="26" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -2093,9 +2095,9 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="19"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="22"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="9" t="s">
         <v>15</v>
       </c>
@@ -2110,9 +2112,9 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="19"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="22"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="9" t="s">
         <v>16</v>
       </c>
@@ -2125,9 +2127,9 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="19"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="22"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="27"/>
       <c r="D67" s="9" t="s">
         <v>4</v>
       </c>
@@ -2138,9 +2140,9 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="19"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="23"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="28"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -2151,9 +2153,9 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="19"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="15" t="s">
+      <c r="A69" s="24"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -2166,9 +2168,9 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="19"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="24"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="17"/>
       <c r="D70" s="9" t="s">
         <v>15</v>
       </c>
@@ -2179,9 +2181,9 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="19"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="24"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="17"/>
       <c r="D71" s="9" t="s">
         <v>16</v>
       </c>
@@ -2192,9 +2194,9 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="19"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="24"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="17"/>
       <c r="D72" s="9" t="s">
         <v>4</v>
       </c>
@@ -2205,9 +2207,9 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="19"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="24"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="17"/>
       <c r="D73" s="6" t="s">
         <v>5</v>
       </c>
@@ -2218,9 +2220,9 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="19"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="15" t="s">
+      <c r="A74" s="24"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -2236,9 +2238,9 @@
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="19"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="24"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="17"/>
       <c r="D75" s="9" t="s">
         <v>15</v>
       </c>
@@ -2252,9 +2254,9 @@
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="19"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="24"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="17"/>
       <c r="D76" s="9" t="s">
         <v>16</v>
       </c>
@@ -2268,9 +2270,9 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="19"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="24"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="17"/>
       <c r="D77" s="9" t="s">
         <v>4</v>
       </c>
@@ -2284,9 +2286,9 @@
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="20"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="25"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="9" t="s">
         <v>5</v>
       </c>
@@ -2464,21 +2466,7 @@
       <c r="I94" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="J38:J41"/>
+  <mergeCells count="31">
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="B44:B78"/>
     <mergeCell ref="A44:A78"/>
@@ -2495,6 +2483,21 @@
     <mergeCell ref="A3:A42"/>
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="C18:C22"/>
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="J38:J41"/>
+    <mergeCell ref="J33:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Done 75% of the module with calendar
</commit_message>
<xml_diff>
--- a/ClickNStyle Documents/System Status  and Info.xlsx
+++ b/ClickNStyle Documents/System Status  and Info.xlsx
@@ -672,6 +672,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -679,63 +736,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
@@ -1036,28 +1036,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="30">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1081,13 +1081,13 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="29">
         <v>42672</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1101,14 +1101,14 @@
         <v>23</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="24"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1122,12 +1122,12 @@
         <v>23</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="24"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
@@ -1137,12 +1137,12 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="24"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1152,12 +1152,12 @@
       </c>
       <c r="G6" s="9"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="15"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1170,9 +1170,9 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="24"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -1184,14 +1184,14 @@
         <v>23</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="24"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
@@ -1205,12 +1205,12 @@
         <v>23</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="24"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
@@ -1224,12 +1224,12 @@
         <v>23</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="24"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1239,12 +1239,12 @@
         <v>23</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="24"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,9 +1257,9 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="24"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1271,14 +1271,14 @@
         <v>23</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="24"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1292,13 +1292,13 @@
         <v>23</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="24"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1312,12 +1312,12 @@
         <v>23</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="24"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
@@ -1327,12 +1327,12 @@
         <v>23</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="24"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
@@ -1345,9 +1345,9 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="24"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1359,14 +1359,14 @@
         <v>23</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="24"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="9" t="s">
         <v>15</v>
       </c>
@@ -1380,12 +1380,12 @@
         <v>23</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="14"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="24"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1397,12 +1397,12 @@
         <v>23</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="24"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
@@ -1412,12 +1412,12 @@
         <v>23</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="15"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="24"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="9" t="s">
         <v>5</v>
       </c>
@@ -1430,9 +1430,9 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="24"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="16" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1444,14 +1444,14 @@
         <v>23</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="24"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
@@ -1465,12 +1465,12 @@
         <v>23</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="14"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="24"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="9" t="s">
         <v>16</v>
       </c>
@@ -1482,12 +1482,12 @@
         <v>23</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="24"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
@@ -1497,12 +1497,12 @@
         <v>23</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="24"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="9" t="s">
         <v>5</v>
       </c>
@@ -1515,9 +1515,9 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="24"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="16" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1529,14 +1529,14 @@
         <v>23</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="24"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1550,12 +1550,12 @@
         <v>23</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="14"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="24"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="9" t="s">
         <v>16</v>
       </c>
@@ -1565,12 +1565,12 @@
         <v>23</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="14"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="24"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
@@ -1580,12 +1580,12 @@
         <v>23</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="15"/>
+      <c r="J31" s="34"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="24"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="9" t="s">
         <v>5</v>
       </c>
@@ -1598,9 +1598,9 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="24"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="16" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -1612,14 +1612,14 @@
         <v>23</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="24"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="9" t="s">
         <v>15</v>
       </c>
@@ -1631,12 +1631,12 @@
         <v>23</v>
       </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="14"/>
+      <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="24"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="9" t="s">
         <v>16</v>
       </c>
@@ -1646,12 +1646,12 @@
         <v>23</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="14"/>
+      <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="24"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="9" t="s">
         <v>4</v>
       </c>
@@ -1661,12 +1661,12 @@
         <v>23</v>
       </c>
       <c r="I36" s="1"/>
-      <c r="J36" s="15"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="24"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="9" t="s">
         <v>5</v>
       </c>
@@ -1679,9 +1679,9 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="24"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="16" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -1693,14 +1693,14 @@
         <v>23</v>
       </c>
       <c r="I38" s="1"/>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="24"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1710,12 +1710,12 @@
         <v>23</v>
       </c>
       <c r="I39" s="1"/>
-      <c r="J39" s="14"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="24"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="17"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="9" t="s">
         <v>16</v>
       </c>
@@ -1725,12 +1725,12 @@
         <v>23</v>
       </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="14"/>
+      <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="24"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
@@ -1740,12 +1740,12 @@
         <v>23</v>
       </c>
       <c r="I41" s="1"/>
-      <c r="J41" s="15"/>
+      <c r="J41" s="34"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="25"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -1780,13 +1780,13 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -1801,9 +1801,9 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="24"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="9" t="s">
         <v>15</v>
       </c>
@@ -1820,9 +1820,9 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="24"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="9" t="s">
         <v>16</v>
       </c>
@@ -1835,9 +1835,9 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="24"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="17"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="9" t="s">
         <v>4</v>
       </c>
@@ -1852,9 +1852,9 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="24"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="17"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -1865,9 +1865,9 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="24"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="16" t="s">
+      <c r="A49" s="19"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -1880,9 +1880,9 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="24"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="17"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="9" t="s">
         <v>15</v>
       </c>
@@ -1895,9 +1895,9 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="24"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="17"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="9" t="s">
         <v>16</v>
       </c>
@@ -1908,9 +1908,9 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="24"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="17"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="9" t="s">
         <v>4</v>
       </c>
@@ -1921,9 +1921,9 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="24"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="17"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="6" t="s">
         <v>5</v>
       </c>
@@ -1934,9 +1934,9 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="24"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="16" t="s">
+      <c r="A54" s="19"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -1951,9 +1951,9 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="24"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="24"/>
       <c r="D55" s="9" t="s">
         <v>15</v>
       </c>
@@ -1968,9 +1968,9 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="24"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="17"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="24"/>
       <c r="D56" s="9" t="s">
         <v>16</v>
       </c>
@@ -1985,9 +1985,9 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="24"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="17"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="24"/>
       <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
@@ -2000,9 +2000,9 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="24"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="17"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
@@ -2013,9 +2013,9 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="24"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="16" t="s">
+      <c r="A59" s="19"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -2028,9 +2028,9 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="24"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="17"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="9" t="s">
         <v>15</v>
       </c>
@@ -2041,9 +2041,9 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="24"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="17"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="9" t="s">
         <v>16</v>
       </c>
@@ -2054,9 +2054,9 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="24"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="17"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="9" t="s">
         <v>4</v>
       </c>
@@ -2067,9 +2067,9 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="24"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="17"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2080,9 +2080,9 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="24"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="26" t="s">
+      <c r="A64" s="19"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -2095,9 +2095,9 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="24"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="27"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="9" t="s">
         <v>15</v>
       </c>
@@ -2112,9 +2112,9 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="24"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="9" t="s">
         <v>16</v>
       </c>
@@ -2127,9 +2127,9 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="24"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="9" t="s">
         <v>4</v>
       </c>
@@ -2140,9 +2140,9 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="24"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="28"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="23"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -2153,9 +2153,9 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="24"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="16" t="s">
+      <c r="A69" s="19"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15" t="s">
         <v>32</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -2168,9 +2168,9 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="24"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="17"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="24"/>
       <c r="D70" s="9" t="s">
         <v>15</v>
       </c>
@@ -2181,9 +2181,9 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="24"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="24"/>
       <c r="D71" s="9" t="s">
         <v>16</v>
       </c>
@@ -2194,9 +2194,9 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="24"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="17"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="24"/>
       <c r="D72" s="9" t="s">
         <v>4</v>
       </c>
@@ -2207,9 +2207,9 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="24"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="17"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="24"/>
       <c r="D73" s="6" t="s">
         <v>5</v>
       </c>
@@ -2220,9 +2220,9 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="24"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="16" t="s">
+      <c r="A74" s="19"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -2238,9 +2238,9 @@
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="24"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="17"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="9" t="s">
         <v>15</v>
       </c>
@@ -2254,9 +2254,9 @@
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="24"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="17"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="24"/>
       <c r="D76" s="9" t="s">
         <v>16</v>
       </c>
@@ -2270,9 +2270,9 @@
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="24"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="17"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="24"/>
       <c r="D77" s="9" t="s">
         <v>4</v>
       </c>
@@ -2286,9 +2286,9 @@
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="25"/>
-      <c r="B78" s="22"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="9" t="s">
         <v>5</v>
       </c>
@@ -2467,6 +2467,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="J38:J41"/>
+    <mergeCell ref="J33:J36"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="B44:B78"/>
     <mergeCell ref="A44:A78"/>
@@ -2483,21 +2498,6 @@
     <mergeCell ref="A3:A42"/>
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="J38:J41"/>
-    <mergeCell ref="J33:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>